<commit_message>
update lake and the alum data path
</commit_message>
<xml_diff>
--- a/NeapWorkflow_GET_MarineTerrestrial_Extant-2010_250m.xlsx
+++ b/NeapWorkflow_GET_MarineTerrestrial_Extant-2010_250m.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\new298\OneDrive - CSIRO\Code\Python\NEAP\ecosystem-typology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2455D874-A69F-4CDE-BE62-450C51B0FBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37388BE1-1CDE-4240-AE85-335255DA062B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>epsg:4283</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\NLUM_ALUMV8_250m_2010_11_alb\NLUM_ALUMV8_250m_2010_11_alb.tif</t>
-  </si>
-  <si>
     <t>NN</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>https://github.com/CSIRO-enviro-informatics/ecosystem-typology/raw/main/crosswalks/Geofabric-IUCNGET/Lacustrine-IUCNGET.xlsx</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240723.shp</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\Terrestrial_Extant_EPSG3577_250m.tif</t>
   </si>
   <si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_IUCNGET_DK_20240801.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2010_11_to_2020_21_prerelease3_20240809\NLUM_v7p3_ALUMV8_250m_2010_11_alb\NLUM_v7p3_ALUMV8_250m_2010_11_alb.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240808_NoOverlapWithALUM.shp</t>
   </si>
 </sst>
 </file>
@@ -533,36 +533,36 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="136.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="105.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="112.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -571,13 +571,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -586,18 +586,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -612,7 +612,7 @@
         <v>18</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -621,18 +621,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -647,7 +647,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
@@ -656,18 +656,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -682,24 +682,24 @@
         <v>18</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -711,19 +711,19 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -731,10 +731,10 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -746,10 +746,10 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
         <v>13</v>
@@ -758,18 +758,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -778,13 +778,13 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -802,11 +802,10 @@
     <hyperlink ref="I3" r:id="rId5" xr:uid="{07B7F3B9-7ED0-459D-A5AD-E62B86EC2810}"/>
     <hyperlink ref="B2" r:id="rId6" xr:uid="{4AAD34BE-AFA6-4C42-98A5-31EBD33DB2C2}"/>
     <hyperlink ref="J5" r:id="rId7" xr:uid="{9D2ED58A-1BCA-4AFA-A7DB-AC11216EF831}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{6D271174-0A26-4C2B-8A49-23E0D84CB50C}"/>
-    <hyperlink ref="I4" r:id="rId9" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
-    <hyperlink ref="B4" r:id="rId10" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
+    <hyperlink ref="I4" r:id="rId8" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>